<commit_message>
GPLIM-3088: when validating headers report all unknown header names at once rather than one error per upload attempt
</commit_message>
<xml_diff>
--- a/mercury/src/test/resources/testdata/manifest-upload/manifest-with-missing-column.xlsx
+++ b/mercury/src/test/resources/testdata/manifest-upload/manifest-with-missing-column.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="1680" yWindow="1680" windowWidth="23920" windowHeight="14380"/>
@@ -33,153 +33,78 @@
     <t>Visit</t>
   </si>
   <si>
-    <t>03101231193</t>
-  </si>
-  <si>
     <t>10-May-2010</t>
   </si>
   <si>
     <t>Screening</t>
   </si>
   <si>
-    <t>03101067213</t>
-  </si>
-  <si>
     <t>25-Feb-2010</t>
   </si>
   <si>
-    <t>03101214167</t>
-  </si>
-  <si>
     <t>02-Mar-2010</t>
   </si>
   <si>
-    <t>03101067211</t>
-  </si>
-  <si>
     <t>14-Oct-2009</t>
   </si>
   <si>
-    <t>03101989209</t>
-  </si>
-  <si>
     <t>29-Aug-2012</t>
   </si>
   <si>
-    <t>03101947686</t>
-  </si>
-  <si>
     <t>16-Aug-2012</t>
   </si>
   <si>
-    <t>03101892406</t>
-  </si>
-  <si>
     <t>03-May-2012</t>
   </si>
   <si>
-    <t>03101757212</t>
-  </si>
-  <si>
     <t>03-Feb-2012</t>
   </si>
   <si>
-    <t>03101064137</t>
-  </si>
-  <si>
     <t>09-Apr-2010</t>
   </si>
   <si>
-    <t>03101231191</t>
-  </si>
-  <si>
     <t>21-Sep-2010</t>
   </si>
   <si>
-    <t>03102000417</t>
-  </si>
-  <si>
     <t>07-Sep-2012</t>
   </si>
   <si>
-    <t>03102000418</t>
-  </si>
-  <si>
     <t>24-Sep-2012</t>
   </si>
   <si>
-    <t>03101752021</t>
-  </si>
-  <si>
     <t>08-Feb-2012</t>
   </si>
   <si>
-    <t>03101752020</t>
-  </si>
-  <si>
     <t>22-Dec-2011</t>
   </si>
   <si>
-    <t>03101411324</t>
-  </si>
-  <si>
     <t>14-Sep-2010</t>
   </si>
   <si>
-    <t>03101411323</t>
-  </si>
-  <si>
     <t>01-Dec-2010</t>
   </si>
   <si>
-    <t>03101492492</t>
-  </si>
-  <si>
     <t>20-Jul-2011</t>
   </si>
   <si>
-    <t>03101492495</t>
-  </si>
-  <si>
     <t>18-Jul-2011</t>
   </si>
   <si>
-    <t>03101254358</t>
-  </si>
-  <si>
     <t>06-May-2010</t>
   </si>
   <si>
-    <t>03101254357</t>
-  </si>
-  <si>
     <t>03-Sep-2010</t>
   </si>
   <si>
-    <t>03101254356</t>
-  </si>
-  <si>
     <t>07-May-2010</t>
   </si>
   <si>
-    <t>03101170867</t>
-  </si>
-  <si>
     <t>05-Feb-2010</t>
   </si>
   <si>
-    <t>03101778110</t>
-  </si>
-  <si>
     <t>24-Apr-2012</t>
   </si>
   <si>
-    <t>T/N</t>
-  </si>
-  <si>
-    <t>Sample ID</t>
-  </si>
-  <si>
     <t>Male</t>
   </si>
   <si>
@@ -190,6 +115,81 @@
   </si>
   <si>
     <t>Normal</t>
+  </si>
+  <si>
+    <t>Patient_ID</t>
+  </si>
+  <si>
+    <t>SAMPLE_TYPE</t>
+  </si>
+  <si>
+    <t>004-002</t>
+  </si>
+  <si>
+    <t>001-001</t>
+  </si>
+  <si>
+    <t>001-002</t>
+  </si>
+  <si>
+    <t>002-003</t>
+  </si>
+  <si>
+    <t>003-009</t>
+  </si>
+  <si>
+    <t>003-008</t>
+  </si>
+  <si>
+    <t>003-007</t>
+  </si>
+  <si>
+    <t>003-006</t>
+  </si>
+  <si>
+    <t>003-001</t>
+  </si>
+  <si>
+    <t>003-002</t>
+  </si>
+  <si>
+    <t>005-013</t>
+  </si>
+  <si>
+    <t>005-014</t>
+  </si>
+  <si>
+    <t>005-012</t>
+  </si>
+  <si>
+    <t>005-011</t>
+  </si>
+  <si>
+    <t>005-005</t>
+  </si>
+  <si>
+    <t>005-007</t>
+  </si>
+  <si>
+    <t>005-010</t>
+  </si>
+  <si>
+    <t>005-009</t>
+  </si>
+  <si>
+    <t>005-002</t>
+  </si>
+  <si>
+    <t>005-004</t>
+  </si>
+  <si>
+    <t>005-003</t>
+  </si>
+  <si>
+    <t>006-001</t>
+  </si>
+  <si>
+    <t>009-001</t>
   </si>
 </sst>
 </file>
@@ -658,20 +658,19 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -683,398 +682,398 @@
         <v>2</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="2" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="2" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="2" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="2" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="2" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="2" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="2" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="2" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="2" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" s="5" t="s">
         <v>30</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="2" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="2" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="2" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="2" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="2" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="2" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="2" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="2" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="2" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>